<commit_message>
Refactor - complete bovine lentivirus extension
</commit_message>
<xml_diff>
--- a/tabular/core/lenti-core-reference-data.xlsx
+++ b/tabular/core/lenti-core-reference-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/retrovirus/Lentivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAF0587-6620-8346-9DE9-43014B453B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356CD8FD-75E9-244E-8E78-75500CFC8980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2360" yWindow="2180" windowWidth="38620" windowHeight="24740" xr2:uid="{FE909052-171A-A641-A05A-6F5B3D043973}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="81">
   <si>
     <t>sequenceID</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Small ruminant lentivirus genotype A</t>
   </si>
   <si>
-    <t>SRLV-A</t>
-  </si>
-  <si>
     <t>SRLV</t>
   </si>
   <si>
@@ -186,9 +183,6 @@
     <t>Human immunodeficiency virus 1</t>
   </si>
   <si>
-    <t>HIV-1M</t>
-  </si>
-  <si>
     <t xml:space="preserve">HIV-1 </t>
   </si>
   <si>
@@ -282,19 +276,7 @@
     <t>Small ruminant lentivirus genotypeB3</t>
   </si>
   <si>
-    <t>SRLV-B</t>
-  </si>
-  <si>
-    <t>SRLV-G</t>
-  </si>
-  <si>
-    <t>SRLV-E1</t>
-  </si>
-  <si>
-    <t>SRLV-E2</t>
-  </si>
-  <si>
-    <t>SRLV-B3</t>
+    <t>HIV-1</t>
   </si>
 </sst>
 </file>
@@ -746,7 +728,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="F5" sqref="A1:N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,35 +827,35 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="K3" s="3" t="s">
         <v>22</v>
       </c>
@@ -881,7 +863,7 @@
         <v>22</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>22</v>
@@ -889,19 +871,19 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>18</v>
@@ -913,11 +895,11 @@
         <v>18</v>
       </c>
       <c r="I4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="K4" s="8" t="s">
         <v>22</v>
       </c>
@@ -925,7 +907,7 @@
         <v>22</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N4" s="8" t="s">
         <v>22</v>
@@ -933,43 +915,43 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="F5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="H5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="J5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="N5" s="10" t="s">
         <v>22</v>
@@ -977,19 +959,19 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>19</v>
@@ -998,13 +980,13 @@
         <v>19</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>22</v>
@@ -1030,34 +1012,34 @@
         <v>26</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="F7" s="8">
         <v>1</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="8">
         <v>1</v>
       </c>
       <c r="I7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="K7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="N7" s="8" t="s">
         <v>22</v>
@@ -1065,43 +1047,43 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="F8" s="8">
         <v>1</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H8" s="9">
         <v>1</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L8" s="8">
         <v>1974</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N8" s="10" t="s">
         <v>22</v>
@@ -1109,43 +1091,43 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="F9" s="8">
         <v>3</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H9" s="9">
         <v>3</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>22</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N9" s="10" t="s">
         <v>22</v>
@@ -1153,43 +1135,43 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="F10" s="8">
         <v>1</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H10" s="9">
         <v>1</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>22</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N10" s="10" t="s">
         <v>22</v>
@@ -1197,43 +1179,43 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="F11" s="8">
         <v>2</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H11" s="9">
         <v>2</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>22</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N11" s="10" t="s">
         <v>22</v>
@@ -1241,43 +1223,43 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="F12" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H12" s="9">
         <v>1</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K12" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="N12" s="10" t="s">
         <v>22</v>

</xml_diff>